<commit_message>
Finito Funziona ( problemi con i tempi)
</commit_message>
<xml_diff>
--- a/link_fonti.xlsx
+++ b/link_fonti.xlsx
@@ -4,7 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Foglio1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Foglio2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,21 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Links</t>
+  </si>
   <si>
     <t>https://www.studenti.it/brigate-rosse-storia-attentati.html</t>
   </si>
   <si>
-    <t>URL</t>
+    <t>https://it.wikipedia.org/wiki/Anni_di_piombo</t>
   </si>
   <si>
-    <t>https://www.focus.it/cultura/storia/terrorismo-rosso-anni-di-piombo</t>
+    <t>https://www.sissco.it/recensione-annale/il-mondo-della-guerra-fredda-e-litalia-degli-anni-di-piombo-una-regia-internazionale-per-il-terrorismo/</t>
   </si>
   <si>
-    <t>https://www.skuola.net/storia-contemporanea/italia-gruppi-terroristici-anni-settanta.html</t>
-  </si>
-  <si>
-    <t>https://www.politicasemplice.it/capire-politica/concetti-fondamentali/cosa-sono-destra-sinistra-oggi-italia/</t>
+    <t>https://www.storicang.it/a/lomicidio-di-aldo-moro_15532</t>
   </si>
 </sst>
 </file>
@@ -41,13 +40,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <u/>
@@ -134,25 +134,25 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -199,7 +199,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Foglio2-style">
+    <tableStyle count="3" pivot="0" name="Foglio1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -212,16 +212,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A15" displayName="Tabella_1" name="Tabella_1" id="1">
   <tableColumns count="1">
-    <tableColumn name="URL" id="1"/>
+    <tableColumn name="Links" id="1"/>
   </tableColumns>
-  <tableStyleInfo name="Foglio2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Foglio1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -425,29 +421,6 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="A1"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
@@ -455,31 +428,31 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="22.63"/>
+    <col customWidth="1" min="1" max="2" width="22.63"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>